<commit_message>
Archon Event Base Release
</commit_message>
<xml_diff>
--- a/document/sample/app/locale.xlsx
+++ b/document/sample/app/locale.xlsx
@@ -61,7 +61,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -93,9 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -403,12 +404,12 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
     <col min="2" max="4" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>